<commit_message>
working on new report module
</commit_message>
<xml_diff>
--- a/application/views/plugins/reports/Sell_analyse/Sell_analyse.xlsx
+++ b/application/views/plugins/reports/Sell_analyse/Sell_analyse.xlsx
@@ -357,16 +357,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3"/>
+  <dimension ref="B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>